<commit_message>
Selesai buat import data pegawai
</commit_message>
<xml_diff>
--- a/src/SIAkademik/SIAkademik.Web/wwwroot/file/importTemplate/Template Import Data Siswa.xlsx
+++ b/src/SIAkademik/SIAkademik.Web/wwwroot/file/importTemplate/Template Import Data Siswa.xlsx
@@ -1249,8 +1249,8 @@
   <sheetPr/>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1660,21 +1660,21 @@
       <c r="J31" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1" insertRows="0" deleteRows="0" objects="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DuTllhESsqNG36pvsSYT6iWqNQKw+gWPVHUZeymNh8ClAK24sn/QOM9DdOyE9zDvtVrfYhWz3mRUtuDnpMbynw==" saltValue="0GutEf1gxPxeihavFQc07Q==" spinCount="100000" sheet="1" selectLockedCells="1" insertRows="0" deleteRows="0" objects="1"/>
   <protectedRanges>
     <protectedRange sqref="A2:J1048576" name="Range1" securityDescriptor="O:WDG:WDD:"/>
   </protectedRanges>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30 D31 D2:D29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
       <formula1>"KristenProtestan,Katolik,Islam,Hindu,Budha,Konghucu,KepercayanTuhanYangMahaEsa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E30 E31 E2:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31">
       <formula1>"LakiLaki,Perempuan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I30 I31 I2:I29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I31">
       <formula1>"Aktif,TidakAktif"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J30 J31 J2:J29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J31">
       <formula1>"X,XI,XII"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>